<commit_message>
Found AprilTag Field Constants for WORLDS Day 1 and puts the spreadsheet in the right place
</commit_message>
<xml_diff>
--- a/RoboCode/src/main/java/us/brainstormz/localizer/aprilTagLocalization/Find AprilTag Calibration.xlsx
+++ b/RoboCode/src/main/java/us/brainstormz/localizer/aprilTagLocalization/Find AprilTag Calibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/RoboCode/src/main/java/us/brainstormz/localizer/aprilTagLocalization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D85638-8250-BB4A-BE78-0AF11B9CF437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB242B72-10EA-C145-BBC8-8E7A7BF0C9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="14660" activeTab="8" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Worlds-like test" sheetId="8" r:id="rId8"/>
+    <sheet name="WORLDS Right" sheetId="8" r:id="rId8"/>
+    <sheet name="WORLDS Left" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="119">
   <si>
     <t>Point</t>
   </si>
@@ -479,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,9 +492,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4780,8 +4778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A25" zoomScale="83" workbookViewId="0">
+      <selection sqref="A1:M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4821,10 +4819,10 @@
         <v>107</v>
       </c>
       <c r="B2" s="1">
-        <v>47.94</v>
+        <v>47.21</v>
       </c>
       <c r="C2" s="1">
-        <v>-44.63</v>
+        <v>-44.88</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="8">
@@ -4834,15 +4832,15 @@
         <v>47.625</v>
       </c>
       <c r="K2">
-        <f xml:space="preserve"> E2 - ABS(B2)</f>
-        <v>-0.43999999999999773</v>
+        <f t="shared" ref="K2:L5" si="0" xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>0.28999999999999915</v>
       </c>
       <c r="L2">
-        <f xml:space="preserve"> F2 - ABS(C2)</f>
-        <v>2.9949999999999974</v>
+        <f t="shared" si="0"/>
+        <v>2.7449999999999974</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
+        <f t="shared" ref="M2" si="1" xml:space="preserve"> G2 - ABS(D2)</f>
         <v>0</v>
       </c>
     </row>
@@ -4851,10 +4849,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>23.66</v>
+        <v>23.42</v>
       </c>
       <c r="C3" s="1">
-        <v>-44.53</v>
+        <v>-44.82</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="8">
@@ -4868,15 +4866,15 @@
         <v>0.625</v>
       </c>
       <c r="K3">
-        <f xml:space="preserve"> E3 - ABS(B3)</f>
-        <v>-3.5000000000000142E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.20499999999999829</v>
       </c>
       <c r="L3">
-        <f xml:space="preserve"> F3 - ABS(C3)</f>
-        <v>3.0949999999999989</v>
+        <f t="shared" si="0"/>
+        <v>2.8049999999999997</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M6" si="1" xml:space="preserve"> G3 - ABS(D3)</f>
+        <f t="shared" ref="M3:M5" si="2" xml:space="preserve"> G3 - ABS(D3)</f>
         <v>0</v>
       </c>
     </row>
@@ -4885,10 +4883,10 @@
         <v>108</v>
       </c>
       <c r="B4" s="1">
-        <v>48.69</v>
+        <v>47.5</v>
       </c>
       <c r="C4" s="1">
-        <v>-20.55</v>
+        <v>-21.18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="8">
@@ -4898,15 +4896,15 @@
         <v>23.875</v>
       </c>
       <c r="K4">
-        <f xml:space="preserve"> E4 - ABS(B4)</f>
-        <v>-1.1899999999999977</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="L4">
-        <f xml:space="preserve"> F4 - ABS(C4)</f>
-        <v>3.3249999999999993</v>
+        <f t="shared" si="0"/>
+        <v>2.6950000000000003</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4915,10 +4913,10 @@
         <v>109</v>
       </c>
       <c r="B5" s="1">
-        <v>23.26</v>
+        <v>23.06</v>
       </c>
       <c r="C5" s="1">
-        <v>-20.350000000000001</v>
+        <v>-21.13</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="8">
@@ -4928,47 +4926,24 @@
         <v>23.875</v>
       </c>
       <c r="K5">
-        <f xml:space="preserve"> E5 - ABS(B5)</f>
-        <v>0.48999999999999844</v>
+        <f t="shared" si="0"/>
+        <v>0.69000000000000128</v>
       </c>
       <c r="L5">
-        <f xml:space="preserve"> F5 - ABS(C5)</f>
-        <v>3.5249999999999986</v>
+        <f t="shared" si="0"/>
+        <v>2.745000000000001</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -4987,9 +4962,6 @@
       <c r="F8" s="1">
         <v>23.375</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="1"/>
@@ -5019,11 +4991,11 @@
       <c r="F11" s="1"/>
       <c r="K11">
         <f>AVERAGE(K2:K5)</f>
-        <v>-0.29374999999999929</v>
+        <v>0.29624999999999968</v>
       </c>
       <c r="L11">
         <f>AVERAGE(L2:L5)</f>
-        <v>3.2349999999999985</v>
+        <v>2.7474999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -5046,11 +5018,11 @@
     <row r="14" spans="1:13">
       <c r="K14">
         <f>K2-$K$11</f>
-        <v>-0.14624999999999844</v>
+        <v>-6.2500000000005329E-3</v>
       </c>
       <c r="L14">
         <f>L2-$L$11</f>
-        <v>-0.2400000000000011</v>
+        <v>-2.5000000000021672E-3</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -5061,41 +5033,41 @@
       <c r="F15" s="9"/>
       <c r="K15">
         <f>K3-$K$11</f>
-        <v>0.25874999999999915</v>
+        <v>-9.1250000000001386E-2</v>
       </c>
       <c r="L15">
         <f>L3-$L$11</f>
-        <v>-0.13999999999999968</v>
+        <v>5.7500000000000107E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="K16">
         <f>K4-$K$11</f>
-        <v>-0.89624999999999844</v>
+        <v>-0.29624999999999968</v>
       </c>
       <c r="L16">
         <f>L4-$L$11</f>
-        <v>9.0000000000000746E-2</v>
+        <v>-5.2499999999999325E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="K17">
         <f>K5-$K$11</f>
-        <v>0.78374999999999773</v>
+        <v>0.3937500000000016</v>
       </c>
       <c r="L17">
         <f>L5-$L$11</f>
-        <v>0.29000000000000004</v>
+        <v>-2.4999999999986144E-3</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="O20">
         <f>K46-K11</f>
-        <v>0.30625000000000036</v>
+        <v>6.6250000000001918E-2</v>
       </c>
       <c r="P20">
         <f>L11-L46</f>
-        <v>-0.91500000000000092</v>
+        <v>0.26250000000000107</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -5120,10 +5092,10 @@
         <v>112</v>
       </c>
       <c r="B30" s="1">
-        <v>-23.34</v>
+        <v>-23.49</v>
       </c>
       <c r="C30" s="1">
-        <v>43.9</v>
+        <v>-44.95</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="8">
@@ -5133,15 +5105,15 @@
         <v>47.625</v>
       </c>
       <c r="K30">
-        <f xml:space="preserve"> E30 - ABS(B30)</f>
-        <v>0.53500000000000014</v>
+        <f t="shared" ref="K30:L33" si="3" xml:space="preserve"> E30 - ABS(B30)</f>
+        <v>0.38500000000000156</v>
       </c>
       <c r="L30">
-        <f xml:space="preserve"> F30 - ABS(C30)</f>
-        <v>3.7250000000000014</v>
+        <f t="shared" si="3"/>
+        <v>2.6749999999999972</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M33" si="2" xml:space="preserve"> G30 - ABS(D30)</f>
+        <f t="shared" ref="M30:M33" si="4" xml:space="preserve"> G30 - ABS(D30)</f>
         <v>0</v>
       </c>
     </row>
@@ -5150,10 +5122,10 @@
         <v>113</v>
       </c>
       <c r="B31" s="1">
-        <v>-47.48</v>
+        <v>-47.4</v>
       </c>
       <c r="C31" s="1">
-        <v>-44.45</v>
+        <v>-44.99</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="8">
@@ -5163,15 +5135,15 @@
         <v>47.625</v>
       </c>
       <c r="K31">
-        <f xml:space="preserve"> E31 - ABS(B31)</f>
-        <v>0.14500000000000313</v>
+        <f t="shared" si="3"/>
+        <v>0.22500000000000142</v>
       </c>
       <c r="L31">
-        <f xml:space="preserve"> F31 - ABS(C31)</f>
-        <v>3.1749999999999972</v>
+        <f t="shared" si="3"/>
+        <v>2.634999999999998</v>
       </c>
       <c r="M31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5180,10 +5152,10 @@
         <v>114</v>
       </c>
       <c r="B32" s="1">
-        <v>-24.44</v>
+        <v>-23.25</v>
       </c>
       <c r="C32" s="1">
-        <v>-18.46</v>
+        <v>-21.16</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="8">
@@ -5193,15 +5165,15 @@
         <v>23.375</v>
       </c>
       <c r="K32">
-        <f xml:space="preserve"> E32 - ABS(B32)</f>
-        <v>-0.56500000000000128</v>
+        <f t="shared" si="3"/>
+        <v>0.625</v>
       </c>
       <c r="L32">
-        <f xml:space="preserve"> F32 - ABS(C32)</f>
-        <v>4.9149999999999991</v>
+        <f t="shared" si="3"/>
+        <v>2.2149999999999999</v>
       </c>
       <c r="M32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5210,10 +5182,10 @@
         <v>115</v>
       </c>
       <c r="B33" s="1">
-        <v>-47.69</v>
+        <v>-47.41</v>
       </c>
       <c r="C33" s="1">
-        <v>-18.59</v>
+        <v>-20.96</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="8">
@@ -5223,29 +5195,24 @@
         <v>23.375</v>
       </c>
       <c r="K33">
-        <f xml:space="preserve"> E33 - ABS(B33)</f>
-        <v>-6.4999999999997726E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.21500000000000341</v>
       </c>
       <c r="L33">
-        <f xml:space="preserve"> F33 - ABS(C33)</f>
-        <v>4.7850000000000001</v>
+        <f t="shared" si="3"/>
+        <v>2.4149999999999991</v>
       </c>
       <c r="M33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
     </row>
     <row r="36" spans="1:13">
       <c r="B36" s="1"/>
@@ -5264,55 +5231,550 @@
     <row r="46" spans="1:13">
       <c r="K46">
         <f>AVERAGE(K30:K33)</f>
-        <v>1.2500000000001066E-2</v>
+        <v>0.3625000000000016</v>
       </c>
       <c r="L46">
         <f>AVERAGE(L30:L33)</f>
-        <v>4.1499999999999995</v>
+        <v>2.4849999999999985</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="K48">
         <f>K30-$K$46</f>
-        <v>0.52249999999999908</v>
+        <v>2.2499999999999964E-2</v>
       </c>
       <c r="L48">
         <f>L30-$L$46</f>
-        <v>-0.42499999999999805</v>
+        <v>0.18999999999999861</v>
       </c>
     </row>
     <row r="49" spans="11:12">
       <c r="K49">
         <f>K31-$K$46</f>
-        <v>0.13250000000000206</v>
+        <v>-0.13750000000000018</v>
       </c>
       <c r="L49">
         <f>L31-$L$46</f>
-        <v>-0.97500000000000231</v>
+        <v>0.14999999999999947</v>
       </c>
     </row>
     <row r="50" spans="11:12">
       <c r="K50">
         <f>K32-$K$46</f>
-        <v>-0.57750000000000234</v>
+        <v>0.2624999999999984</v>
       </c>
       <c r="L50">
         <f>L32-$L$46</f>
-        <v>0.76499999999999968</v>
+        <v>-0.26999999999999869</v>
       </c>
     </row>
     <row r="51" spans="11:12">
       <c r="K51">
         <f>K33-$K$46</f>
-        <v>-7.7499999999998792E-2</v>
+        <v>-0.14749999999999819</v>
       </c>
       <c r="L51">
         <f>L33-$L$46</f>
-        <v>0.63500000000000068</v>
+        <v>-6.9999999999999396E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF693B-9F4C-BF45-B022-47F0F12E085E}">
+  <dimension ref="A1:M51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1">
+        <v>47.19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-44.83</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="8">
+        <v>47.5</v>
+      </c>
+      <c r="F2" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:M5" si="0" xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>0.31000000000000227</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>2.7950000000000017</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1">
+        <v>23.28</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-44.91</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="8">
+        <v>23.625</v>
+      </c>
+      <c r="F3" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="H3">
+        <f>5/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0.34499999999999886</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>2.7150000000000034</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1">
+        <v>47.33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-21.02</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="8">
+        <v>47.5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>23.875</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0.17000000000000171</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>2.8550000000000004</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1">
+        <v>22.72</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-20.99</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="8">
+        <v>23.75</v>
+      </c>
+      <c r="F5" s="8">
+        <v>23.875</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1.0300000000000011</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>2.8850000000000016</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-20.6</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>15.625</v>
+      </c>
+      <c r="F8" s="1">
+        <v>23.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="K10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="K11">
+        <f>AVERAGE(K2:K5)</f>
+        <v>0.46375000000000099</v>
+      </c>
+      <c r="L11">
+        <f>AVERAGE(L2:L5)</f>
+        <v>2.8125000000000018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="K13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="K14">
+        <f>K2-$K$11</f>
+        <v>-0.15374999999999872</v>
+      </c>
+      <c r="L14">
+        <f>L2-$L$11</f>
+        <v>-1.7500000000000071E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="K15">
+        <f>K3-$K$11</f>
+        <v>-0.11875000000000213</v>
+      </c>
+      <c r="L15">
+        <f>L3-$L$11</f>
+        <v>-9.7499999999998366E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="K16">
+        <f>K4-$K$11</f>
+        <v>-0.29374999999999929</v>
+      </c>
+      <c r="L16">
+        <f>L4-$L$11</f>
+        <v>4.249999999999865E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="K17">
+        <f>K5-$K$11</f>
+        <v>0.56625000000000014</v>
+      </c>
+      <c r="L17">
+        <f>L5-$L$11</f>
+        <v>7.2499999999999787E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="K28" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="H29">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-23.62</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-44.78</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="8">
+        <v>23.875</v>
+      </c>
+      <c r="F30" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ref="K30:M33" si="1" xml:space="preserve"> E30 - ABS(B30)</f>
+        <v>0.25499999999999901</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>2.8449999999999989</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="1">
+        <v>-47.62</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-44.96</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="F31" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>5.000000000002558E-3</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>2.6649999999999991</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="1">
+        <v>-23.29</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-20.91</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="8">
+        <v>23.875</v>
+      </c>
+      <c r="F32" s="8">
+        <v>23.375</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0.58500000000000085</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-46.94</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-20.47</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="8">
+        <v>47.625</v>
+      </c>
+      <c r="F33" s="8">
+        <v>23.375</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0.68500000000000227</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>2.9050000000000011</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="K45" t="s">
+        <v>110</v>
+      </c>
+      <c r="L45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="K46">
+        <f>AVERAGE(K30:K33)</f>
+        <v>0.38250000000000117</v>
+      </c>
+      <c r="L46">
+        <f>AVERAGE(L30:L33)</f>
+        <v>2.7199999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="K48">
+        <f>K30-$K$46</f>
+        <v>-0.12750000000000217</v>
+      </c>
+      <c r="L48">
+        <f>L30-$L$46</f>
+        <v>0.12499999999999911</v>
+      </c>
+    </row>
+    <row r="49" spans="11:12">
+      <c r="K49">
+        <f>K31-$K$46</f>
+        <v>-0.37749999999999861</v>
+      </c>
+      <c r="L49">
+        <f>L31-$L$46</f>
+        <v>-5.5000000000000604E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="11:12">
+      <c r="K50">
+        <f>K32-$K$46</f>
+        <v>0.20249999999999968</v>
+      </c>
+      <c r="L50">
+        <f>L32-$L$46</f>
+        <v>-0.25499999999999989</v>
+      </c>
+    </row>
+    <row r="51" spans="11:12">
+      <c r="K51">
+        <f>K33-$K$46</f>
+        <v>0.3025000000000011</v>
+      </c>
+      <c r="L51">
+        <f>L33-$L$46</f>
+        <v>0.18500000000000139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>